<commit_message>
refactor and add support to include all fields
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Product-2023-09-08" r:id="rId3" sheetId="1"/>
+    <sheet name="Product-2023-09-09" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -50,13 +50,13 @@
     <t>Product A</t>
   </si>
   <si>
-    <t>08/09/2023 01:34</t>
-  </si>
-  <si>
-    <t>08 sept. 2023</t>
-  </si>
-  <si>
-    <t>2023-09-08T01:34:07.1482443+01:00[Africa/Casablanca]</t>
+    <t>09/09/2023 17:45</t>
+  </si>
+  <si>
+    <t>09 sept. 2023</t>
+  </si>
+  <si>
+    <t>2023-09-09T17:45:19.6415433+01:00[Africa/Casablanca]</t>
   </si>
   <si>
     <t>A</t>

</xml_diff>

<commit_message>
refactor and try to fix tests
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -50,13 +50,13 @@
     <t>Product A</t>
   </si>
   <si>
-    <t>09/09/2023 17:45</t>
+    <t>09/09/2023 17:59</t>
   </si>
   <si>
     <t>09 sept. 2023</t>
   </si>
   <si>
-    <t>2023-09-09T17:45:19.6415433+01:00[Africa/Casablanca]</t>
+    <t>2023-09-09T17:59:14.0171641+01:00[Africa/Casablanca]</t>
   </si>
   <si>
     <t>A</t>

</xml_diff>

<commit_message>
try to fix tests
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -50,13 +50,13 @@
     <t>Product A</t>
   </si>
   <si>
-    <t>09/09/2023 17:59</t>
+    <t>09/09/2023 18:12</t>
   </si>
   <si>
     <t>09 sept. 2023</t>
   </si>
   <si>
-    <t>2023-09-09T17:59:14.0171641+01:00[Africa/Casablanca]</t>
+    <t>2023-09-09T18:12:25.0708549+01:00[Africa/Casablanca]</t>
   </si>
   <si>
     <t>A</t>

</xml_diff>

<commit_message>
remove constructor annotations, add enumvalues annotation, refactor
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Product-2023-09-10" r:id="rId3" sheetId="1"/>
+    <sheet name="Product-2023-09-11" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>name</t>
   </si>
@@ -50,22 +50,19 @@
     <t>Product A</t>
   </si>
   <si>
-    <t>10/09/2023 02:19</t>
-  </si>
-  <si>
-    <t>2023-09-10</t>
-  </si>
-  <si>
-    <t>2023-09-10T02:19:50.0570456+01:00[Africa/Casablanca]</t>
-  </si>
-  <si>
-    <t>A</t>
+    <t>11/09/2023 00:33</t>
+  </si>
+  <si>
+    <t>2023-09-11</t>
+  </si>
+  <si>
+    <t>2023-09-11T00:33:09.7899063+01:00[Africa/Casablanca]</t>
+  </si>
+  <si>
+    <t>bb</t>
   </si>
   <si>
     <t>Product B</t>
-  </si>
-  <si>
-    <t>B</t>
   </si>
 </sst>
 </file>
@@ -247,7 +244,7 @@
         <v>14</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixes,handle the case when only certain columns need to be mapped
</commit_message>
<xml_diff>
--- a/src/test/resources/products.xlsx
+++ b/src/test/resources/products.xlsx
@@ -6,7 +6,7 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Product-2023-09-11" r:id="rId3" sheetId="1"/>
+    <sheet name="Product-2023-09-12" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
@@ -20,7 +20,7 @@
     <t>price</t>
   </si>
   <si>
-    <t>promo price</t>
+    <t>Promo price</t>
   </si>
   <si>
     <t>min price</t>
@@ -53,19 +53,19 @@
     <t>Product A</t>
   </si>
   <si>
-    <t>11/09/2023 14:57</t>
-  </si>
-  <si>
-    <t>2023-09-11</t>
-  </si>
-  <si>
-    <t>2023-09-11T14:57:29.2342794+01:00[Africa/Casablanca]</t>
+    <t>12/09/2023 00:17</t>
+  </si>
+  <si>
+    <t>2023-09-12</t>
+  </si>
+  <si>
+    <t>2023-09-12T00:17:58.4095525+01:00[Africa/Casablanca]</t>
   </si>
   <si>
     <t>bb</t>
   </si>
   <si>
-    <t>2023-09-11T14:57:29.2342794</t>
+    <t>2023-09-12T00:17:58.4095525</t>
   </si>
   <si>
     <t>Product B</t>
@@ -137,7 +137,7 @@
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="9.8515625"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="5.79296875"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.5703125"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.68359375"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="9.90234375"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="6.68359375"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="8.125"/>

</xml_diff>